<commit_message>
New code and data file
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Entered</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Homework</t>
   </si>
   <si>
-    <t>22-10-2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Woon-werk (heen en terug)</t>
   </si>
   <si>
@@ -57,25 +54,20 @@
     <t>None</t>
   </si>
   <si>
-    <t>23-10-2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maastricht, Paul Henri Spaaklaan</t>
   </si>
   <si>
-    <t>24-10-2025</t>
-  </si>
-  <si>
     <t>Thuiswerkvergoeding</t>
-  </si>
-  <si>
-    <t>25-10-2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.000000"/>
@@ -104,12 +96,15 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,12 +609,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="2" max="2" width="9.8515625"/>
+    <col bestFit="1" min="2" max="2" style="1" width="21.421875"/>
     <col bestFit="1" customWidth="1" min="3" max="3" width="24.140625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" width="13.421875"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="14.140625"/>
     <col bestFit="1" min="6" max="6" width="28.8515625"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" width="19.00390625"/>
+    <col customWidth="1" min="7" max="7" width="21.57421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -632,7 +627,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -646,96 +641,408 @@
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4">
+        <v>45940</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45941</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="2">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="3">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="4">
+        <v>45942</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="2">
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="3">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B5" s="4">
+        <v>45943</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" ht="14.25">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" ht="14.25">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" ht="14.25">
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" ht="14.25">
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" ht="14.25">
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" ht="14.25">
+      <c r="B53" s="5"/>
+    </row>
+    <row r="54" ht="14.25">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" ht="14.25">
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" ht="14.25">
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" ht="14.25">
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" ht="14.25">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" ht="14.25">
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" ht="14.25">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" ht="14.25">
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" ht="14.25">
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" ht="14.25">
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" ht="14.25">
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" ht="14.25">
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" ht="14.25">
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" ht="14.25">
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" ht="14.25">
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" ht="14.25">
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" ht="14.25">
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" ht="14.25">
+      <c r="B73" s="5"/>
+    </row>
+    <row r="74" ht="14.25">
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" ht="14.25">
+      <c r="B75" s="5"/>
+    </row>
+    <row r="76" ht="14.25">
+      <c r="B76" s="5"/>
+    </row>
+    <row r="77" ht="14.25">
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" ht="14.25">
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" ht="14.25">
+      <c r="B79" s="5"/>
+    </row>
+    <row r="80" ht="14.25">
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" ht="14.25">
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" ht="14.25">
+      <c r="B82" s="5"/>
+    </row>
+    <row r="83" ht="14.25">
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" ht="14.25">
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" ht="14.25">
+      <c r="B85" s="5"/>
+    </row>
+    <row r="86" ht="14.25">
+      <c r="B86" s="5"/>
+    </row>
+    <row r="87" ht="14.25">
+      <c r="B87" s="5"/>
+    </row>
+    <row r="88" ht="14.25">
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" ht="14.25">
+      <c r="B89" s="5"/>
+    </row>
+    <row r="90" ht="14.25">
+      <c r="B90" s="5"/>
+    </row>
+    <row r="91" ht="14.25">
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" ht="14.25">
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" ht="14.25">
+      <c r="B93" s="5"/>
+    </row>
+    <row r="94" ht="14.25">
+      <c r="B94" s="5"/>
+    </row>
+    <row r="95" ht="14.25">
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" ht="14.25">
+      <c r="B96" s="5"/>
+    </row>
+    <row r="97" ht="14.25">
+      <c r="B97" s="5"/>
+    </row>
+    <row r="98" ht="14.25">
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" ht="14.25">
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" ht="14.25">
+      <c r="B100" s="5"/>
+    </row>
+    <row r="101" ht="14.25">
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" ht="14.25">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" ht="14.25">
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" ht="14.25">
+      <c r="B104" s="5"/>
+    </row>
+    <row r="105" ht="14.25">
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" ht="14.25">
+      <c r="B106" s="5"/>
+    </row>
+    <row r="107" ht="14.25">
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" ht="14.25">
+      <c r="B108" s="5"/>
+    </row>
+    <row r="109" ht="14.25">
+      <c r="B109" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>